<commit_message>
Added 2nd result within TeachingLab Four bar
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/Experimental/CoolTerm/result2.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/Experimental/CoolTerm/result2.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\Experimental\CoolTerm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA5EFC7-14C1-4600-8A22-FCAFE0D8A0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3B4E9C-6FAE-4D7C-9AE9-4AE8E0E4756D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12096" tabRatio="500" xr2:uid="{841305C8-7A9F-47AF-8AED-1298C162DFB0}"/>
+    <workbookView xWindow="3015" yWindow="1620" windowWidth="21600" windowHeight="11295" xr2:uid="{BD00F354-5689-413C-B6A1-62F752553B6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sep 4 Trial" sheetId="1" r:id="rId1"/>
+    <sheet name="Sep 4 Trial (2)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Time Stamp</t>
-  </si>
-  <si>
-    <t>Time (msec)</t>
   </si>
   <si>
     <t>Hall Sensor</t>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>Time (msec)</t>
   </si>
 </sst>
 </file>
@@ -226,9 +229,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -258,12 +277,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -271,15 +284,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -585,89 +589,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
-    <a:spDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
       <a:lstStyle/>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
     </a:lnDef>
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
@@ -680,152 +619,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5204AB0D-8214-4A3A-AF95-F93C6374BC9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E89836B-0D89-4366-99B0-62BD3B01D8F4}">
   <dimension ref="A1:S342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="7.44140625" customWidth="1"/>
-    <col min="3" max="7" width="5.5546875" customWidth="1"/>
+    <col min="1" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" customWidth="1"/>
-    <col min="11" max="13" width="5.5546875" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="11" max="13" width="5.7109375" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
-    <col min="16" max="16" width="6.5546875" customWidth="1"/>
-    <col min="17" max="19" width="5.5546875" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="19" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="16"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="10"/>
-    </row>
-    <row r="2" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="18"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="13" t="s">
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="15"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17" t="s">
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="17" t="s">
+      <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="Q3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="12" t="s">
+      <c r="R3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>68315</v>
       </c>
       <c r="B4">
-        <f>A4-$A$4</f>
+        <f>A4-68315</f>
         <v>0</v>
       </c>
       <c r="C4">
@@ -880,12 +819,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>68421</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B68" si="0">A5-$A$4</f>
+        <f t="shared" ref="B5:B68" si="0">A5-68315</f>
         <v>106</v>
       </c>
       <c r="C5">
@@ -940,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>68529</v>
       </c>
@@ -1000,7 +939,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>68636</v>
       </c>
@@ -1060,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>68744</v>
       </c>
@@ -1120,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>68850</v>
       </c>
@@ -1180,7 +1119,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>68956</v>
       </c>
@@ -1240,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>69061</v>
       </c>
@@ -1300,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>69165</v>
       </c>
@@ -1360,67 +1299,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>69269</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
         <v>954</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
         <v>-0.54</v>
       </c>
-      <c r="E13">
-        <v>0.12</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="F13" s="4">
         <v>9.17</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <v>0.25</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>0.75</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <v>0.06</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>3.19</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
         <v>359.94</v>
       </c>
-      <c r="O13">
-        <v>0.12</v>
-      </c>
-      <c r="P13">
+      <c r="O13" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="P13" s="4">
         <v>-6.19</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
+      <c r="R13" s="4">
+        <v>0</v>
+      </c>
+      <c r="S13" s="4">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>69372</v>
       </c>
@@ -1480,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>69479</v>
       </c>
@@ -1540,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>69584</v>
       </c>
@@ -1600,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>69692</v>
       </c>
@@ -1660,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>69798</v>
       </c>
@@ -1720,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>69904</v>
       </c>
@@ -1780,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>70012</v>
       </c>
@@ -1840,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>70120</v>
       </c>
@@ -1900,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>70227</v>
       </c>
@@ -1960,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>70336</v>
       </c>
@@ -2020,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>70444</v>
       </c>
@@ -2080,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>70551</v>
       </c>
@@ -2140,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>70658</v>
       </c>
@@ -2200,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>70764</v>
       </c>
@@ -2260,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>70872</v>
       </c>
@@ -2320,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>70977</v>
       </c>
@@ -2380,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>71085</v>
       </c>
@@ -2440,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>71192</v>
       </c>
@@ -2500,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>71300</v>
       </c>
@@ -2560,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>71408</v>
       </c>
@@ -2620,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>71516</v>
       </c>
@@ -2680,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>71624</v>
       </c>
@@ -2740,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>71731</v>
       </c>
@@ -2800,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>71836</v>
       </c>
@@ -2860,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>71942</v>
       </c>
@@ -2920,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>72047</v>
       </c>
@@ -2980,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>72154</v>
       </c>
@@ -3040,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>72261</v>
       </c>
@@ -3100,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>72367</v>
       </c>
@@ -3160,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>72474</v>
       </c>
@@ -3220,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>72580</v>
       </c>
@@ -3280,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>72687</v>
       </c>
@@ -3340,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>72794</v>
       </c>
@@ -3400,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>72899</v>
       </c>
@@ -3460,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>73006</v>
       </c>
@@ -3520,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>73110</v>
       </c>
@@ -3580,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>73213</v>
       </c>
@@ -3640,7 +3579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>73317</v>
       </c>
@@ -3700,7 +3639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>73420</v>
       </c>
@@ -3760,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>73525</v>
       </c>
@@ -3820,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>73628</v>
       </c>
@@ -3880,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>73735</v>
       </c>
@@ -3940,7 +3879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>73840</v>
       </c>
@@ -4000,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>73946</v>
       </c>
@@ -4060,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>74050</v>
       </c>
@@ -4120,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>74157</v>
       </c>
@@ -4180,7 +4119,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>74263</v>
       </c>
@@ -4240,7 +4179,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>74370</v>
       </c>
@@ -4300,7 +4239,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>74478</v>
       </c>
@@ -4360,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>74586</v>
       </c>
@@ -4420,7 +4359,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>74693</v>
       </c>
@@ -4480,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>74799</v>
       </c>
@@ -4540,7 +4479,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>74904</v>
       </c>
@@ -4600,67 +4539,67 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="67" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
         <v>75009</v>
       </c>
       <c r="B67">
         <f t="shared" si="0"/>
         <v>6694</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-      <c r="D67">
+      <c r="C67" s="4">
+        <v>0</v>
+      </c>
+      <c r="D67" s="4">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="4">
         <v>0.02</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="4">
         <v>7.85</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="4">
         <v>0.15</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="4">
         <v>0.88</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="4">
         <v>0.06</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="4">
         <v>4.4400000000000004</v>
       </c>
-      <c r="K67">
+      <c r="K67" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="4">
         <v>-0.01</v>
       </c>
-      <c r="M67">
-        <v>0</v>
-      </c>
-      <c r="N67">
+      <c r="M67" s="4">
+        <v>0</v>
+      </c>
+      <c r="N67" s="4">
         <v>359.94</v>
       </c>
-      <c r="O67">
-        <v>0.12</v>
-      </c>
-      <c r="P67">
+      <c r="O67" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="P67" s="4">
         <v>-4.63</v>
       </c>
-      <c r="Q67">
+      <c r="Q67" s="4">
         <v>0.63</v>
       </c>
-      <c r="R67">
-        <v>0</v>
-      </c>
-      <c r="S67">
+      <c r="R67" s="4">
+        <v>0</v>
+      </c>
+      <c r="S67" s="4">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>75112</v>
       </c>
@@ -4720,12 +4659,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>75217</v>
       </c>
       <c r="B69">
-        <f t="shared" ref="B69:B132" si="1">A69-$A$4</f>
+        <f t="shared" ref="B69:B132" si="1">A69-68315</f>
         <v>6902</v>
       </c>
       <c r="C69">
@@ -4780,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>75326</v>
       </c>
@@ -4840,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>75432</v>
       </c>
@@ -4900,7 +4839,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>75540</v>
       </c>
@@ -4960,7 +4899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>75649</v>
       </c>
@@ -5020,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>75758</v>
       </c>
@@ -5080,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>75868</v>
       </c>
@@ -5140,7 +5079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75975</v>
       </c>
@@ -5200,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76085</v>
       </c>
@@ -5260,7 +5199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76192</v>
       </c>
@@ -5320,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>76299</v>
       </c>
@@ -5380,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>76406</v>
       </c>
@@ -5440,7 +5379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>76513</v>
       </c>
@@ -5500,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>76619</v>
       </c>
@@ -5560,7 +5499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>76726</v>
       </c>
@@ -5620,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>76830</v>
       </c>
@@ -5680,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>76938</v>
       </c>
@@ -5740,7 +5679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>77045</v>
       </c>
@@ -5800,7 +5739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>77155</v>
       </c>
@@ -5860,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>77263</v>
       </c>
@@ -5920,7 +5859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>77372</v>
       </c>
@@ -5980,7 +5919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>77480</v>
       </c>
@@ -6040,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>77587</v>
       </c>
@@ -6100,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>77692</v>
       </c>
@@ -6160,7 +6099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>77799</v>
       </c>
@@ -6220,7 +6159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>77904</v>
       </c>
@@ -6280,7 +6219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>78012</v>
       </c>
@@ -6340,7 +6279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>78118</v>
       </c>
@@ -6400,7 +6339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>78226</v>
       </c>
@@ -6460,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>78332</v>
       </c>
@@ -6520,7 +6459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>78438</v>
       </c>
@@ -6580,7 +6519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>78545</v>
       </c>
@@ -6640,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>78652</v>
       </c>
@@ -6700,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>78756</v>
       </c>
@@ -6760,7 +6699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>78862</v>
       </c>
@@ -6820,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>78965</v>
       </c>
@@ -6880,7 +6819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>79069</v>
       </c>
@@ -6940,7 +6879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>79171</v>
       </c>
@@ -7000,7 +6939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>79273</v>
       </c>
@@ -7060,7 +6999,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>79377</v>
       </c>
@@ -7120,7 +7059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>79482</v>
       </c>
@@ -7180,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>79588</v>
       </c>
@@ -7240,7 +7179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>79691</v>
       </c>
@@ -7300,7 +7239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>79797</v>
       </c>
@@ -7360,7 +7299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>79901</v>
       </c>
@@ -7420,7 +7359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>80008</v>
       </c>
@@ -7480,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>80116</v>
       </c>
@@ -7540,7 +7479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>80223</v>
       </c>
@@ -7600,7 +7539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>80328</v>
       </c>
@@ -7660,7 +7599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>80434</v>
       </c>
@@ -7720,7 +7659,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>80539</v>
       </c>
@@ -7780,7 +7719,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>80644</v>
       </c>
@@ -7840,7 +7779,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>80747</v>
       </c>
@@ -7900,7 +7839,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>80851</v>
       </c>
@@ -7960,7 +7899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>80953</v>
       </c>
@@ -8020,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>81059</v>
       </c>
@@ -8080,7 +8019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>81167</v>
       </c>
@@ -8140,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>81274</v>
       </c>
@@ -8200,7 +8139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>81381</v>
       </c>
@@ -8260,7 +8199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>81486</v>
       </c>
@@ -8320,7 +8259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>81595</v>
       </c>
@@ -8380,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>81702</v>
       </c>
@@ -8440,7 +8379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>81811</v>
       </c>
@@ -8500,7 +8439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>81918</v>
       </c>
@@ -8560,12 +8499,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>82024</v>
       </c>
       <c r="B133">
-        <f t="shared" ref="B133:B196" si="2">A133-$A$4</f>
+        <f t="shared" ref="B133:B196" si="2">A133-68315</f>
         <v>13709</v>
       </c>
       <c r="C133">
@@ -8620,7 +8559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>82130</v>
       </c>
@@ -8680,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>82236</v>
       </c>
@@ -8740,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>82341</v>
       </c>
@@ -8800,7 +8739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>82448</v>
       </c>
@@ -8860,7 +8799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>82553</v>
       </c>
@@ -8920,7 +8859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>82660</v>
       </c>
@@ -8980,7 +8919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>82766</v>
       </c>
@@ -9040,7 +8979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>82873</v>
       </c>
@@ -9100,7 +9039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>82980</v>
       </c>
@@ -9160,7 +9099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>83087</v>
       </c>
@@ -9220,7 +9159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>83194</v>
       </c>
@@ -9280,7 +9219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>83300</v>
       </c>
@@ -9340,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>83405</v>
       </c>
@@ -9400,7 +9339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>83510</v>
       </c>
@@ -9460,7 +9399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>83614</v>
       </c>
@@ -9520,7 +9459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>83721</v>
       </c>
@@ -9580,7 +9519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>83827</v>
       </c>
@@ -9640,7 +9579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>83933</v>
       </c>
@@ -9700,7 +9639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>84038</v>
       </c>
@@ -9760,7 +9699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>84144</v>
       </c>
@@ -9820,7 +9759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>84250</v>
       </c>
@@ -9880,7 +9819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>84357</v>
       </c>
@@ -9940,7 +9879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>84463</v>
       </c>
@@ -10000,7 +9939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>84566</v>
       </c>
@@ -10060,7 +9999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>84670</v>
       </c>
@@ -10120,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>84769</v>
       </c>
@@ -10180,7 +10119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>84872</v>
       </c>
@@ -10240,7 +10179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>84973</v>
       </c>
@@ -10300,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>85073</v>
       </c>
@@ -10360,7 +10299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>85176</v>
       </c>
@@ -10420,7 +10359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>85278</v>
       </c>
@@ -10480,7 +10419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>85383</v>
       </c>
@@ -10540,7 +10479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>85486</v>
       </c>
@@ -10600,7 +10539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>85591</v>
       </c>
@@ -10660,7 +10599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>85696</v>
       </c>
@@ -10720,7 +10659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>85801</v>
       </c>
@@ -10780,7 +10719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>85908</v>
       </c>
@@ -10840,7 +10779,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>86013</v>
       </c>
@@ -10900,7 +10839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>86120</v>
       </c>
@@ -10960,7 +10899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>86225</v>
       </c>
@@ -11020,7 +10959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>86331</v>
       </c>
@@ -11080,7 +11019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>86435</v>
       </c>
@@ -11140,7 +11079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>86538</v>
       </c>
@@ -11200,7 +11139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>86643</v>
       </c>
@@ -11260,7 +11199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>86747</v>
       </c>
@@ -11320,7 +11259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>86854</v>
       </c>
@@ -11380,7 +11319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>86960</v>
       </c>
@@ -11440,7 +11379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>87067</v>
       </c>
@@ -11500,7 +11439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>87175</v>
       </c>
@@ -11560,7 +11499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>87281</v>
       </c>
@@ -11620,7 +11559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>87390</v>
       </c>
@@ -11680,7 +11619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>87497</v>
       </c>
@@ -11740,7 +11679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>87605</v>
       </c>
@@ -11800,7 +11739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>87712</v>
       </c>
@@ -11860,7 +11799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>87819</v>
       </c>
@@ -11920,7 +11859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>87925</v>
       </c>
@@ -11980,7 +11919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>88031</v>
       </c>
@@ -12040,7 +11979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>88136</v>
       </c>
@@ -12100,7 +12039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>88243</v>
       </c>
@@ -12160,7 +12099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>88348</v>
       </c>
@@ -12220,7 +12159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>88456</v>
       </c>
@@ -12280,7 +12219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>88563</v>
       </c>
@@ -12340,7 +12279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>88671</v>
       </c>
@@ -12400,12 +12339,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>88778</v>
       </c>
       <c r="B197">
-        <f t="shared" ref="B197:B260" si="3">A197-$A$4</f>
+        <f t="shared" ref="B197:B260" si="3">A197-68315</f>
         <v>20463</v>
       </c>
       <c r="C197">
@@ -12460,7 +12399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>88885</v>
       </c>
@@ -12520,7 +12459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>88992</v>
       </c>
@@ -12580,7 +12519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>89100</v>
       </c>
@@ -12640,7 +12579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>89206</v>
       </c>
@@ -12700,7 +12639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>89314</v>
       </c>
@@ -12760,7 +12699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>89421</v>
       </c>
@@ -12820,7 +12759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>89527</v>
       </c>
@@ -12880,7 +12819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>89632</v>
       </c>
@@ -12940,7 +12879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>89736</v>
       </c>
@@ -13000,7 +12939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>89842</v>
       </c>
@@ -13060,7 +12999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>89947</v>
       </c>
@@ -13120,7 +13059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>90053</v>
       </c>
@@ -13180,7 +13119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>90159</v>
       </c>
@@ -13240,7 +13179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>90264</v>
       </c>
@@ -13300,7 +13239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>90369</v>
       </c>
@@ -13360,7 +13299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>90470</v>
       </c>
@@ -13420,7 +13359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>90573</v>
       </c>
@@ -13480,7 +13419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>90674</v>
       </c>
@@ -13540,7 +13479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>90776</v>
       </c>
@@ -13600,7 +13539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>90876</v>
       </c>
@@ -13660,7 +13599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>90979</v>
       </c>
@@ -13720,7 +13659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>91082</v>
       </c>
@@ -13780,7 +13719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>91189</v>
       </c>
@@ -13840,7 +13779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>91294</v>
       </c>
@@ -13900,7 +13839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>91401</v>
       </c>
@@ -13960,7 +13899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>91507</v>
       </c>
@@ -14020,7 +13959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>91613</v>
       </c>
@@ -14080,7 +14019,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>91720</v>
       </c>
@@ -14140,7 +14079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>91826</v>
       </c>
@@ -14200,7 +14139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>91932</v>
       </c>
@@ -14260,7 +14199,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>92039</v>
       </c>
@@ -14320,7 +14259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>92143</v>
       </c>
@@ -14380,7 +14319,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>92248</v>
       </c>
@@ -14440,7 +14379,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>92350</v>
       </c>
@@ -14500,7 +14439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>92455</v>
       </c>
@@ -14560,7 +14499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>92561</v>
       </c>
@@ -14620,7 +14559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>92665</v>
       </c>
@@ -14680,7 +14619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>92773</v>
       </c>
@@ -14740,7 +14679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>92879</v>
       </c>
@@ -14800,7 +14739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>92987</v>
       </c>
@@ -14860,7 +14799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>93095</v>
       </c>
@@ -14920,7 +14859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>93203</v>
       </c>
@@ -14980,7 +14919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>93312</v>
       </c>
@@ -15040,7 +14979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>93419</v>
       </c>
@@ -15100,7 +15039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>93526</v>
       </c>
@@ -15160,7 +15099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>93632</v>
       </c>
@@ -15220,7 +15159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>93737</v>
       </c>
@@ -15280,7 +15219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>93844</v>
       </c>
@@ -15340,7 +15279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>93948</v>
       </c>
@@ -15400,7 +15339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>94054</v>
       </c>
@@ -15460,7 +15399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>94159</v>
       </c>
@@ -15520,7 +15459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>94266</v>
       </c>
@@ -15580,7 +15519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>94373</v>
       </c>
@@ -15640,7 +15579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>94480</v>
       </c>
@@ -15700,7 +15639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>94587</v>
       </c>
@@ -15760,7 +15699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>94695</v>
       </c>
@@ -15820,7 +15759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>94801</v>
       </c>
@@ -15880,7 +15819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>94909</v>
       </c>
@@ -15940,7 +15879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>95015</v>
       </c>
@@ -16000,7 +15939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>95124</v>
       </c>
@@ -16060,7 +15999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>95233</v>
       </c>
@@ -16120,7 +16059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>95339</v>
       </c>
@@ -16180,7 +16119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>95448</v>
       </c>
@@ -16240,12 +16179,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>95554</v>
       </c>
       <c r="B261">
-        <f t="shared" ref="B261:B324" si="4">A261-$A$4</f>
+        <f t="shared" ref="B261:B324" si="4">A261-68315</f>
         <v>27239</v>
       </c>
       <c r="C261">
@@ -16300,7 +16239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>95663</v>
       </c>
@@ -16360,7 +16299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>95769</v>
       </c>
@@ -16420,7 +16359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>95875</v>
       </c>
@@ -16480,7 +16419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>95979</v>
       </c>
@@ -16540,7 +16479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>96081</v>
       </c>
@@ -16600,7 +16539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>96187</v>
       </c>
@@ -16660,7 +16599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>96291</v>
       </c>
@@ -16720,7 +16659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>96394</v>
       </c>
@@ -16780,7 +16719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>96497</v>
       </c>
@@ -16840,7 +16779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>96601</v>
       </c>
@@ -16900,7 +16839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>96705</v>
       </c>
@@ -16960,7 +16899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>96809</v>
       </c>
@@ -17020,7 +16959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>96915</v>
       </c>
@@ -17080,7 +17019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>97020</v>
       </c>
@@ -17140,7 +17079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>97126</v>
       </c>
@@ -17200,7 +17139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>97231</v>
       </c>
@@ -17260,7 +17199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>97337</v>
       </c>
@@ -17320,7 +17259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>97442</v>
       </c>
@@ -17380,7 +17319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>97547</v>
       </c>
@@ -17440,7 +17379,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>97653</v>
       </c>
@@ -17500,7 +17439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>97760</v>
       </c>
@@ -17560,7 +17499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>97865</v>
       </c>
@@ -17620,7 +17559,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>97971</v>
       </c>
@@ -17680,7 +17619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>98074</v>
       </c>
@@ -17740,7 +17679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>98179</v>
       </c>
@@ -17800,7 +17739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>98283</v>
       </c>
@@ -17860,7 +17799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>98390</v>
       </c>
@@ -17920,7 +17859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>98497</v>
       </c>
@@ -17980,7 +17919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>98603</v>
       </c>
@@ -18040,7 +17979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>98710</v>
       </c>
@@ -18100,7 +18039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>98816</v>
       </c>
@@ -18160,7 +18099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>98924</v>
       </c>
@@ -18220,7 +18159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>99032</v>
       </c>
@@ -18280,7 +18219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>99138</v>
       </c>
@@ -18340,7 +18279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>99246</v>
       </c>
@@ -18400,7 +18339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>99353</v>
       </c>
@@ -18460,7 +18399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>99459</v>
       </c>
@@ -18520,7 +18459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>99565</v>
       </c>
@@ -18580,7 +18519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>99671</v>
       </c>
@@ -18640,7 +18579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>99777</v>
       </c>
@@ -18700,7 +18639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>99884</v>
       </c>
@@ -18760,7 +18699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>99990</v>
       </c>
@@ -18820,7 +18759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>100098</v>
       </c>
@@ -18880,7 +18819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>100205</v>
       </c>
@@ -18940,7 +18879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>100314</v>
       </c>
@@ -19000,7 +18939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>100422</v>
       </c>
@@ -19060,7 +18999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>100530</v>
       </c>
@@ -19120,7 +19059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>100638</v>
       </c>
@@ -19180,7 +19119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>100746</v>
       </c>
@@ -19240,7 +19179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>100853</v>
       </c>
@@ -19300,7 +19239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>100962</v>
       </c>
@@ -19360,7 +19299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>101069</v>
       </c>
@@ -19420,7 +19359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>101178</v>
       </c>
@@ -19480,7 +19419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>101287</v>
       </c>
@@ -19540,7 +19479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>101396</v>
       </c>
@@ -19600,7 +19539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>101506</v>
       </c>
@@ -19660,7 +19599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>101616</v>
       </c>
@@ -19720,7 +19659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>101724</v>
       </c>
@@ -19780,7 +19719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>101831</v>
       </c>
@@ -19840,7 +19779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>101938</v>
       </c>
@@ -19900,7 +19839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>102044</v>
       </c>
@@ -19960,7 +19899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>102150</v>
       </c>
@@ -20020,7 +19959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>102253</v>
       </c>
@@ -20080,12 +20019,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>102359</v>
       </c>
       <c r="B325">
-        <f t="shared" ref="B325:B342" si="5">A325-$A$4</f>
+        <f t="shared" ref="B325:B342" si="5">A325-68315</f>
         <v>34044</v>
       </c>
       <c r="C325">
@@ -20140,7 +20079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>102463</v>
       </c>
@@ -20200,7 +20139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>102568</v>
       </c>
@@ -20260,7 +20199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>102674</v>
       </c>
@@ -20320,7 +20259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>102781</v>
       </c>
@@ -20380,7 +20319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>102889</v>
       </c>
@@ -20440,7 +20379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>102994</v>
       </c>
@@ -20500,7 +20439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>103101</v>
       </c>
@@ -20560,7 +20499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>103207</v>
       </c>
@@ -20620,7 +20559,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="334" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>103314</v>
       </c>
@@ -20680,7 +20619,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="335" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>103421</v>
       </c>
@@ -20740,7 +20679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>103527</v>
       </c>
@@ -20800,7 +20739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>103635</v>
       </c>
@@ -20860,7 +20799,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="338" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>103741</v>
       </c>
@@ -20920,7 +20859,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="339" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>103846</v>
       </c>
@@ -20980,7 +20919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>103952</v>
       </c>
@@ -21040,7 +20979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>104057</v>
       </c>
@@ -21100,7 +21039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>104165</v>
       </c>
@@ -21121,9 +21060,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
-    <mergeCell ref="Q2:S2"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:M1"/>
@@ -21132,6 +21069,8 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B1:B3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>